<commit_message>
refreshing original data and saved dataframes after uploading data  wrangling version 4
</commit_message>
<xml_diff>
--- a/CP2_AQ_HOUSTON/00_SavedDataframes/riopa_indoor.xlsx
+++ b/CP2_AQ_HOUSTON/00_SavedDataframes/riopa_indoor.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="265">
   <si>
     <t>linkid</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>home_long</t>
-  </si>
-  <si>
-    <t>geoid</t>
   </si>
   <si>
     <t>TX103110</t>
@@ -1173,13 +1170,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U121"/>
+  <dimension ref="A1:T121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:20">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1237,25 +1234,22 @@
       <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <v>10951</v>
       </c>
       <c r="D2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F2">
         <v>15.2</v>
@@ -1270,7 +1264,7 @@
         <v>36816</v>
       </c>
       <c r="J2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K2">
         <v>21.1</v>
@@ -1296,22 +1290,28 @@
       <c r="R2">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="3" spans="1:21">
+      <c r="S2">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T2">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3" s="1">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>10889</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F3">
         <v>13</v>
@@ -1326,7 +1326,7 @@
         <v>36795</v>
       </c>
       <c r="J3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K3">
         <v>18.33</v>
@@ -1353,21 +1353,21 @@
         <v>482012526001</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:20">
       <c r="A4" s="1">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>10965</v>
       </c>
       <c r="D4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F4">
         <v>9.300000000000001</v>
@@ -1382,7 +1382,7 @@
         <v>36839</v>
       </c>
       <c r="J4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -1409,21 +1409,21 @@
         <v>482012525004</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:20">
       <c r="A5" s="1">
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5">
         <v>10986</v>
       </c>
       <c r="D5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F5">
         <v>17.2</v>
@@ -1438,7 +1438,7 @@
         <v>36875</v>
       </c>
       <c r="J5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K5">
         <v>19.4908</v>
@@ -1465,21 +1465,21 @@
         <v>482012526001</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:20">
       <c r="A6" s="1">
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <v>10982</v>
       </c>
       <c r="D6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F6">
         <v>11.6</v>
@@ -1494,7 +1494,7 @@
         <v>36906</v>
       </c>
       <c r="J6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -1521,21 +1521,21 @@
         <v>482012525004</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:20">
       <c r="A7" s="1">
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7">
         <v>10002</v>
       </c>
       <c r="D7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F7">
         <v>5.1</v>
@@ -1550,7 +1550,7 @@
         <v>36334</v>
       </c>
       <c r="J7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -1576,22 +1576,28 @@
       <c r="R7">
         <v>482014130001</v>
       </c>
-    </row>
-    <row r="8" spans="1:21">
+      <c r="S7">
+        <v>29.69643017826087</v>
+      </c>
+      <c r="T7">
+        <v>-95.44376722608695</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
       <c r="A8" s="1">
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8">
         <v>10042</v>
       </c>
       <c r="D8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F8">
         <v>4.8</v>
@@ -1606,7 +1612,7 @@
         <v>36340</v>
       </c>
       <c r="J8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K8">
         <v>25.07</v>
@@ -1633,21 +1639,21 @@
         <v>482013140003</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:20">
       <c r="A9" s="1">
         <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9">
         <v>10087</v>
       </c>
       <c r="D9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F9">
         <v>5.6</v>
@@ -1662,7 +1668,7 @@
         <v>36369</v>
       </c>
       <c r="J9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K9">
         <v>26.3</v>
@@ -1688,22 +1694,28 @@
       <c r="R9">
         <v>482012533002</v>
       </c>
-    </row>
-    <row r="10" spans="1:21">
+      <c r="S9">
+        <v>29.758572912</v>
+      </c>
+      <c r="T9">
+        <v>-95.06787043999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
       <c r="A10" s="1">
         <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10">
         <v>10082</v>
       </c>
       <c r="D10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F10">
         <v>19.6</v>
@@ -1718,7 +1730,7 @@
         <v>36390</v>
       </c>
       <c r="J10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K10">
         <v>26.41</v>
@@ -1745,21 +1757,21 @@
         <v>482012535004</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:20">
       <c r="A11" s="1">
         <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11">
         <v>10089</v>
       </c>
       <c r="D11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F11">
         <v>13.7</v>
@@ -1774,7 +1786,7 @@
         <v>36390</v>
       </c>
       <c r="J11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K11">
         <v>25.69</v>
@@ -1801,21 +1813,21 @@
         <v>482012537001</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:20">
       <c r="A12" s="1">
         <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12">
         <v>10094</v>
       </c>
       <c r="D12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F12">
         <v>58.2</v>
@@ -1830,7 +1842,7 @@
         <v>36403</v>
       </c>
       <c r="J12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K12">
         <v>24.6051</v>
@@ -1857,21 +1869,21 @@
         <v>482013223001</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:20">
       <c r="A13" s="1">
         <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13">
         <v>10085</v>
       </c>
       <c r="D13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F13">
         <v>28.9</v>
@@ -1886,7 +1898,7 @@
         <v>36403</v>
       </c>
       <c r="J13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K13">
         <v>25.1028</v>
@@ -1913,21 +1925,21 @@
         <v>482013223001</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:20">
       <c r="A14" s="1">
         <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14">
         <v>10005</v>
       </c>
       <c r="D14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F14">
         <v>14.4</v>
@@ -1942,7 +1954,7 @@
         <v>36405</v>
       </c>
       <c r="J14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K14">
         <v>28.3369</v>
@@ -1969,21 +1981,21 @@
         <v>482013223001</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:20">
       <c r="A15" s="1">
         <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>10003</v>
       </c>
       <c r="D15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F15">
         <v>14</v>
@@ -1998,7 +2010,7 @@
         <v>36411</v>
       </c>
       <c r="J15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K15">
         <v>30.46</v>
@@ -2025,21 +2037,21 @@
         <v>482013223001</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:20">
       <c r="A16" s="1">
         <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16">
         <v>10013</v>
       </c>
       <c r="D16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F16">
         <v>22.9</v>
@@ -2054,7 +2066,7 @@
         <v>36411</v>
       </c>
       <c r="J16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K16">
         <v>28.87</v>
@@ -2086,16 +2098,16 @@
         <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17">
         <v>10125</v>
       </c>
       <c r="D17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F17">
         <v>8.4</v>
@@ -2110,7 +2122,7 @@
         <v>36430</v>
       </c>
       <c r="J17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K17">
         <v>23.9</v>
@@ -2142,16 +2154,16 @@
         <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18">
         <v>10119</v>
       </c>
       <c r="D18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F18">
         <v>32</v>
@@ -2166,7 +2178,7 @@
         <v>36437</v>
       </c>
       <c r="J18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K18">
         <v>25.7163</v>
@@ -2198,16 +2210,16 @@
         <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19">
         <v>10144</v>
       </c>
       <c r="D19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F19">
         <v>11</v>
@@ -2222,7 +2234,7 @@
         <v>36446</v>
       </c>
       <c r="J19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -2254,16 +2266,16 @@
         <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20">
         <v>10152</v>
       </c>
       <c r="D20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F20">
         <v>16</v>
@@ -2278,7 +2290,7 @@
         <v>36452</v>
       </c>
       <c r="J20" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K20">
         <v>23.14</v>
@@ -2310,16 +2322,16 @@
         <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21">
         <v>10157</v>
       </c>
       <c r="D21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E21" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F21">
         <v>16.1</v>
@@ -2334,7 +2346,7 @@
         <v>36479</v>
       </c>
       <c r="J21" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K21">
         <v>21.1</v>
@@ -2366,16 +2378,16 @@
         <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22">
         <v>10181</v>
       </c>
       <c r="D22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E22" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F22">
         <v>19</v>
@@ -2390,7 +2402,7 @@
         <v>36495</v>
       </c>
       <c r="J22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K22">
         <v>22.55</v>
@@ -2422,16 +2434,16 @@
         <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23">
         <v>10159</v>
       </c>
       <c r="D23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F23">
         <v>11.8</v>
@@ -2446,7 +2458,7 @@
         <v>36515</v>
       </c>
       <c r="J23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K23">
         <v>20.76</v>
@@ -2478,16 +2490,16 @@
         <v>76</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24">
         <v>10340</v>
       </c>
       <c r="D24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F24">
         <v>6.3</v>
@@ -2502,7 +2514,7 @@
         <v>36528</v>
       </c>
       <c r="J24" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K24">
         <v>23.9768</v>
@@ -2534,16 +2546,16 @@
         <v>79</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25">
         <v>10251</v>
       </c>
       <c r="D25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E25" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F25">
         <v>18</v>
@@ -2558,7 +2570,7 @@
         <v>36530</v>
       </c>
       <c r="J25" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K25">
         <v>23.0962</v>
@@ -2590,16 +2602,16 @@
         <v>82</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26">
         <v>10249</v>
       </c>
       <c r="D26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F26">
         <v>22.3</v>
@@ -2614,7 +2626,7 @@
         <v>36558</v>
       </c>
       <c r="J26" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K26">
         <v>22.7699</v>
@@ -2646,16 +2658,16 @@
         <v>85</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C27">
         <v>10217</v>
       </c>
       <c r="D27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E27" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F27">
         <v>13.3</v>
@@ -2670,7 +2682,7 @@
         <v>36565</v>
       </c>
       <c r="J27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K27">
         <v>21.1</v>
@@ -2702,16 +2714,16 @@
         <v>88</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C28">
         <v>10275</v>
       </c>
       <c r="D28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E28" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F28">
         <v>11.6</v>
@@ -2726,7 +2738,7 @@
         <v>36572</v>
       </c>
       <c r="J28" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K28">
         <v>24.1298</v>
@@ -2758,16 +2770,16 @@
         <v>91</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C29">
         <v>10221</v>
       </c>
       <c r="D29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E29" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F29">
         <v>17</v>
@@ -2782,7 +2794,7 @@
         <v>36570</v>
       </c>
       <c r="J29" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K29">
         <v>24.1536</v>
@@ -2814,16 +2826,16 @@
         <v>94</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30">
         <v>10222</v>
       </c>
       <c r="D30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F30">
         <v>12.2</v>
@@ -2838,7 +2850,7 @@
         <v>36570</v>
       </c>
       <c r="J30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K30">
         <v>23.8387</v>
@@ -2870,16 +2882,16 @@
         <v>97</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C31">
         <v>10272</v>
       </c>
       <c r="D31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E31" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F31">
         <v>7.5</v>
@@ -2894,7 +2906,7 @@
         <v>36572</v>
       </c>
       <c r="J31" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K31">
         <v>23.495</v>
@@ -2926,16 +2938,16 @@
         <v>99</v>
       </c>
       <c r="B32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C32">
         <v>10347</v>
       </c>
       <c r="D32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E32" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F32">
         <v>13.4</v>
@@ -2950,7 +2962,7 @@
         <v>36577</v>
       </c>
       <c r="J32" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K32">
         <v>22.8406</v>
@@ -2977,21 +2989,21 @@
         <v>482012546005</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:20">
       <c r="A33" s="1">
         <v>103</v>
       </c>
       <c r="B33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C33">
         <v>10348</v>
       </c>
       <c r="D33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E33" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F33">
         <v>17</v>
@@ -3006,7 +3018,7 @@
         <v>36577</v>
       </c>
       <c r="J33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K33">
         <v>22.378</v>
@@ -3033,21 +3045,21 @@
         <v>482012545001</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:20">
       <c r="A34" s="1">
         <v>106</v>
       </c>
       <c r="B34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C34">
         <v>10377</v>
       </c>
       <c r="D34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E34" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F34">
         <v>14</v>
@@ -3062,7 +3074,7 @@
         <v>36579</v>
       </c>
       <c r="J34" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K34">
         <v>26.0687</v>
@@ -3089,21 +3101,21 @@
         <v>482012534001</v>
       </c>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:20">
       <c r="A35" s="1">
         <v>112</v>
       </c>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C35">
         <v>10375</v>
       </c>
       <c r="D35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E35" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F35">
         <v>14.6</v>
@@ -3118,7 +3130,7 @@
         <v>36584</v>
       </c>
       <c r="J35" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K35">
         <v>23.1147</v>
@@ -3145,21 +3157,21 @@
         <v>482013203001</v>
       </c>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:20">
       <c r="A36" s="1">
         <v>115</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C36">
         <v>10416</v>
       </c>
       <c r="D36" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E36" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F36">
         <v>7.2</v>
@@ -3174,7 +3186,7 @@
         <v>36598</v>
       </c>
       <c r="J36" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K36">
         <v>21.3312</v>
@@ -3201,21 +3213,21 @@
         <v>482012523003</v>
       </c>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:20">
       <c r="A37" s="1">
         <v>118</v>
       </c>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C37">
         <v>10413</v>
       </c>
       <c r="D37" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E37" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F37">
         <v>7.7</v>
@@ -3230,7 +3242,7 @@
         <v>36598</v>
       </c>
       <c r="J37" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K37">
         <v>21.0381</v>
@@ -3257,21 +3269,21 @@
         <v>482012526001</v>
       </c>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:20">
       <c r="A38" s="1">
         <v>121</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C38">
         <v>10420</v>
       </c>
       <c r="D38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E38" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F38">
         <v>19.1</v>
@@ -3286,7 +3298,7 @@
         <v>36600</v>
       </c>
       <c r="J38" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K38">
         <v>23.1544</v>
@@ -3312,22 +3324,28 @@
       <c r="R38">
         <v>482012524002</v>
       </c>
-    </row>
-    <row r="39" spans="1:18">
+      <c r="S38">
+        <v>29.78980206</v>
+      </c>
+      <c r="T38">
+        <v>-95.16006806</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20">
       <c r="A39" s="1">
         <v>124</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C39">
         <v>10418</v>
       </c>
       <c r="D39" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E39" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F39">
         <v>24.1</v>
@@ -3342,7 +3360,7 @@
         <v>36600</v>
       </c>
       <c r="J39" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K39">
         <v>25.265</v>
@@ -3368,22 +3386,28 @@
       <c r="R39">
         <v>482012333001</v>
       </c>
-    </row>
-    <row r="40" spans="1:18">
+      <c r="S39">
+        <v>29.76006851515152</v>
+      </c>
+      <c r="T39">
+        <v>-95.19600138787879</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20">
       <c r="A40" s="1">
         <v>127</v>
       </c>
       <c r="B40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C40">
         <v>10462</v>
       </c>
       <c r="D40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E40" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F40">
         <v>9</v>
@@ -3398,7 +3422,7 @@
         <v>36605</v>
       </c>
       <c r="J40" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K40">
         <v>23.2338</v>
@@ -3424,22 +3448,28 @@
       <c r="R40">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="41" spans="1:18">
+      <c r="S40">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T40">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20">
       <c r="A41" s="1">
         <v>130</v>
       </c>
       <c r="B41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C41">
         <v>10463</v>
       </c>
       <c r="D41" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E41" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F41">
         <v>4.1</v>
@@ -3454,7 +3484,7 @@
         <v>36605</v>
       </c>
       <c r="J41" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K41">
         <v>24.4254</v>
@@ -3480,22 +3510,28 @@
       <c r="R41">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="42" spans="1:18">
+      <c r="S41">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T41">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20">
       <c r="A42" s="1">
         <v>133</v>
       </c>
       <c r="B42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C42">
         <v>10468</v>
       </c>
       <c r="D42" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E42" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F42">
         <v>13.3</v>
@@ -3510,7 +3546,7 @@
         <v>36607</v>
       </c>
       <c r="J42" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K42">
         <v>21.1</v>
@@ -3536,22 +3572,28 @@
       <c r="R42">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="43" spans="1:18">
+      <c r="S42">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T42">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20">
       <c r="A43" s="1">
         <v>136</v>
       </c>
       <c r="B43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C43">
         <v>10466</v>
       </c>
       <c r="D43" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E43" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F43">
         <v>35.3</v>
@@ -3566,7 +3608,7 @@
         <v>36607</v>
       </c>
       <c r="J43" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K43">
         <v>24.6028</v>
@@ -3592,22 +3634,28 @@
       <c r="R43">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="44" spans="1:18">
+      <c r="S43">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T43">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20">
       <c r="A44" s="1">
         <v>139</v>
       </c>
       <c r="B44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C44">
         <v>10543</v>
       </c>
       <c r="D44" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E44" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F44">
         <v>4.8</v>
@@ -3622,7 +3670,7 @@
         <v>36621</v>
       </c>
       <c r="J44" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K44">
         <v>24.0313</v>
@@ -3649,21 +3697,21 @@
         <v>482012330004</v>
       </c>
     </row>
-    <row r="45" spans="1:18">
+    <row r="45" spans="1:20">
       <c r="A45" s="1">
         <v>142</v>
       </c>
       <c r="B45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C45">
         <v>10477</v>
       </c>
       <c r="D45" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E45" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F45">
         <v>29.1</v>
@@ -3678,7 +3726,7 @@
         <v>36612</v>
       </c>
       <c r="J45" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K45">
         <v>27.1119</v>
@@ -3705,21 +3753,21 @@
         <v>482012526001</v>
       </c>
     </row>
-    <row r="46" spans="1:18">
+    <row r="46" spans="1:20">
       <c r="A46" s="1">
         <v>145</v>
       </c>
       <c r="B46" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C46">
         <v>10469</v>
       </c>
       <c r="D46" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E46" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F46">
         <v>14.9</v>
@@ -3734,7 +3782,7 @@
         <v>36614</v>
       </c>
       <c r="J46" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K46">
         <v>26.4412</v>
@@ -3761,21 +3809,21 @@
         <v>482012523002</v>
       </c>
     </row>
-    <row r="47" spans="1:18">
+    <row r="47" spans="1:20">
       <c r="A47" s="1">
         <v>148</v>
       </c>
       <c r="B47" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C47">
         <v>10472</v>
       </c>
       <c r="D47" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E47" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F47">
         <v>31.6</v>
@@ -3790,7 +3838,7 @@
         <v>36619</v>
       </c>
       <c r="J47" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K47">
         <v>22.8033</v>
@@ -3817,21 +3865,21 @@
         <v>482012526001</v>
       </c>
     </row>
-    <row r="48" spans="1:18">
+    <row r="48" spans="1:20">
       <c r="A48" s="1">
         <v>151</v>
       </c>
       <c r="B48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C48">
         <v>10473</v>
       </c>
       <c r="D48" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E48" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F48">
         <v>14.9</v>
@@ -3846,7 +3894,7 @@
         <v>36619</v>
       </c>
       <c r="J48" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K48">
         <v>18.8607</v>
@@ -3873,21 +3921,21 @@
         <v>482012526001</v>
       </c>
     </row>
-    <row r="49" spans="1:18">
+    <row r="49" spans="1:20">
       <c r="A49" s="1">
         <v>154</v>
       </c>
       <c r="B49" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C49">
         <v>10545</v>
       </c>
       <c r="D49" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E49" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F49">
         <v>11.3</v>
@@ -3902,7 +3950,7 @@
         <v>36621</v>
       </c>
       <c r="J49" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K49">
         <v>23.1874</v>
@@ -3929,21 +3977,21 @@
         <v>482012526001</v>
       </c>
     </row>
-    <row r="50" spans="1:18">
+    <row r="50" spans="1:20">
       <c r="A50" s="1">
         <v>157</v>
       </c>
       <c r="B50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C50">
         <v>10542</v>
       </c>
       <c r="D50" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E50" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F50">
         <v>58.2</v>
@@ -3958,7 +4006,7 @@
         <v>36626</v>
       </c>
       <c r="J50" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K50">
         <v>22.5</v>
@@ -3984,22 +4032,28 @@
       <c r="R50">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="51" spans="1:18">
+      <c r="S50">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T50">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20">
       <c r="A51" s="1">
         <v>160</v>
       </c>
       <c r="B51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C51">
         <v>10594</v>
       </c>
       <c r="D51" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E51" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F51">
         <v>34.8</v>
@@ -4014,7 +4068,7 @@
         <v>36644</v>
       </c>
       <c r="J51" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K51">
         <v>23.4536</v>
@@ -4040,22 +4094,28 @@
       <c r="R51">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="52" spans="1:18">
+      <c r="S51">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T51">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20">
       <c r="A52" s="1">
         <v>163</v>
       </c>
       <c r="B52" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C52">
         <v>10537</v>
       </c>
       <c r="D52" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E52" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F52">
         <v>8</v>
@@ -4070,7 +4130,7 @@
         <v>36628</v>
       </c>
       <c r="J52" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K52">
         <v>23.7225</v>
@@ -4096,22 +4156,28 @@
       <c r="R52">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="53" spans="1:18">
+      <c r="S52">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T52">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20">
       <c r="A53" s="1">
         <v>166</v>
       </c>
       <c r="B53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C53">
         <v>10540</v>
       </c>
       <c r="D53" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E53" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F53">
         <v>13.6</v>
@@ -4126,7 +4192,7 @@
         <v>36633</v>
       </c>
       <c r="J53" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K53">
         <v>23.9931</v>
@@ -4153,21 +4219,21 @@
         <v>482012526001</v>
       </c>
     </row>
-    <row r="54" spans="1:18">
+    <row r="54" spans="1:20">
       <c r="A54" s="1">
         <v>169</v>
       </c>
       <c r="B54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C54">
         <v>10552</v>
       </c>
       <c r="D54" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E54" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F54">
         <v>10.2</v>
@@ -4182,7 +4248,7 @@
         <v>36635</v>
       </c>
       <c r="J54" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K54">
         <v>24.6585</v>
@@ -4209,21 +4275,21 @@
         <v>482012526001</v>
       </c>
     </row>
-    <row r="55" spans="1:18">
+    <row r="55" spans="1:20">
       <c r="A55" s="1">
         <v>172</v>
       </c>
       <c r="B55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C55">
         <v>10555</v>
       </c>
       <c r="D55" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E55" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F55">
         <v>19.4</v>
@@ -4238,7 +4304,7 @@
         <v>36642</v>
       </c>
       <c r="J55" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K55">
         <v>26.3099</v>
@@ -4264,22 +4330,28 @@
       <c r="R55">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="56" spans="1:18">
+      <c r="S55">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T55">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20">
       <c r="A56" s="1">
         <v>178</v>
       </c>
       <c r="B56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C56">
         <v>10599</v>
       </c>
       <c r="D56" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E56" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F56">
         <v>4.2</v>
@@ -4294,7 +4366,7 @@
         <v>36647</v>
       </c>
       <c r="J56" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K56">
         <v>23.5758</v>
@@ -4320,22 +4392,28 @@
       <c r="R56">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="57" spans="1:18">
+      <c r="S56">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T56">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20">
       <c r="A57" s="1">
         <v>181</v>
       </c>
       <c r="B57" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C57">
         <v>10603</v>
       </c>
       <c r="D57" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E57" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F57">
         <v>3</v>
@@ -4350,7 +4428,7 @@
         <v>36647</v>
       </c>
       <c r="J57" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K57">
         <v>23.89</v>
@@ -4377,21 +4455,21 @@
         <v>482012526001</v>
       </c>
     </row>
-    <row r="58" spans="1:18">
+    <row r="58" spans="1:20">
       <c r="A58" s="1">
         <v>184</v>
       </c>
       <c r="B58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C58">
         <v>10606</v>
       </c>
       <c r="D58" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E58" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F58">
         <v>16.2</v>
@@ -4406,7 +4484,7 @@
         <v>36654</v>
       </c>
       <c r="J58" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K58">
         <v>26.3992</v>
@@ -4430,21 +4508,21 @@
         <v>81.9064</v>
       </c>
     </row>
-    <row r="59" spans="1:18">
+    <row r="59" spans="1:20">
       <c r="A59" s="1">
         <v>187</v>
       </c>
       <c r="B59" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C59">
         <v>10608</v>
       </c>
       <c r="D59" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E59" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F59">
         <v>13.4</v>
@@ -4459,7 +4537,7 @@
         <v>36654</v>
       </c>
       <c r="J59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K59">
         <v>26.4258</v>
@@ -4485,22 +4563,28 @@
       <c r="R59">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="60" spans="1:18">
+      <c r="S59">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T59">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20">
       <c r="A60" s="1">
         <v>190</v>
       </c>
       <c r="B60" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C60">
         <v>10602</v>
       </c>
       <c r="D60" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E60" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F60">
         <v>12.3</v>
@@ -4515,7 +4599,7 @@
         <v>36656</v>
       </c>
       <c r="J60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K60">
         <v>24.7305</v>
@@ -4541,22 +4625,28 @@
       <c r="R60">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="61" spans="1:18">
+      <c r="S60">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T60">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20">
       <c r="A61" s="1">
         <v>193</v>
       </c>
       <c r="B61" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C61">
         <v>10610</v>
       </c>
       <c r="D61" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E61" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F61">
         <v>12.4</v>
@@ -4571,7 +4661,7 @@
         <v>36656</v>
       </c>
       <c r="J61" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K61">
         <v>28.64</v>
@@ -4597,22 +4687,28 @@
       <c r="R61">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="62" spans="1:18">
+      <c r="S61">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T61">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20">
       <c r="A62" s="1">
         <v>196</v>
       </c>
       <c r="B62" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C62">
         <v>10640</v>
       </c>
       <c r="D62" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E62" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F62">
         <v>26.5</v>
@@ -4627,7 +4723,7 @@
         <v>36661</v>
       </c>
       <c r="J62" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K62">
         <v>23.5487</v>
@@ -4653,22 +4749,28 @@
       <c r="R62">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="63" spans="1:18">
+      <c r="S62">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T62">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20">
       <c r="A63" s="1">
         <v>199</v>
       </c>
       <c r="B63" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C63">
         <v>10639</v>
       </c>
       <c r="D63" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E63" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F63">
         <v>37.3</v>
@@ -4683,7 +4785,7 @@
         <v>36663</v>
       </c>
       <c r="J63" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K63">
         <v>26.1156</v>
@@ -4709,22 +4811,28 @@
       <c r="R63">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="64" spans="1:18">
+      <c r="S63">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T63">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20">
       <c r="A64" s="1">
         <v>202</v>
       </c>
       <c r="B64" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C64">
         <v>10631</v>
       </c>
       <c r="D64" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E64" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F64">
         <v>12.7</v>
@@ -4739,7 +4847,7 @@
         <v>36682</v>
       </c>
       <c r="J64" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K64">
         <v>26.4379</v>
@@ -4766,21 +4874,21 @@
         <v>482012526001</v>
       </c>
     </row>
-    <row r="65" spans="1:18">
+    <row r="65" spans="1:20">
       <c r="A65" s="1">
         <v>204</v>
       </c>
       <c r="B65" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C65">
         <v>10642</v>
       </c>
       <c r="D65" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E65" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F65">
         <v>10.9</v>
@@ -4795,7 +4903,7 @@
         <v>36682</v>
       </c>
       <c r="J65" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K65">
         <v>24.1808</v>
@@ -4821,22 +4929,28 @@
       <c r="R65">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="66" spans="1:18">
+      <c r="S65">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T65">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20">
       <c r="A66" s="1">
         <v>207</v>
       </c>
       <c r="B66" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C66">
         <v>10634</v>
       </c>
       <c r="D66" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E66" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F66">
         <v>12.3</v>
@@ -4851,7 +4965,7 @@
         <v>36684</v>
       </c>
       <c r="J66" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K66">
         <v>26.3203</v>
@@ -4877,22 +4991,28 @@
       <c r="R66">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="67" spans="1:18">
+      <c r="S66">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T66">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20">
       <c r="A67" s="1">
         <v>210</v>
       </c>
       <c r="B67" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C67">
         <v>10636</v>
       </c>
       <c r="D67" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E67" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F67">
         <v>5.6</v>
@@ -4907,7 +5027,7 @@
         <v>36689</v>
       </c>
       <c r="J67" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K67">
         <v>25.4047</v>
@@ -4934,21 +5054,21 @@
         <v>482013226002</v>
       </c>
     </row>
-    <row r="68" spans="1:18">
+    <row r="68" spans="1:20">
       <c r="A68" s="1">
         <v>213</v>
       </c>
       <c r="B68" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C68">
         <v>10882</v>
       </c>
       <c r="D68" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E68" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F68">
         <v>31.4</v>
@@ -4963,7 +5083,7 @@
         <v>36774</v>
       </c>
       <c r="J68" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K68">
         <v>29.4</v>
@@ -4990,21 +5110,21 @@
         <v>482012526001</v>
       </c>
     </row>
-    <row r="69" spans="1:18">
+    <row r="69" spans="1:20">
       <c r="A69" s="1">
         <v>215</v>
       </c>
       <c r="B69" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C69">
         <v>11074</v>
       </c>
       <c r="D69" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E69" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F69">
         <v>11</v>
@@ -5019,7 +5139,7 @@
         <v>36929</v>
       </c>
       <c r="J69" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K69">
         <v>24.8261</v>
@@ -5033,22 +5153,28 @@
       <c r="R69">
         <v>482014130001</v>
       </c>
-    </row>
-    <row r="70" spans="1:18">
+      <c r="S69">
+        <v>29.69643017826087</v>
+      </c>
+      <c r="T69">
+        <v>-95.44376722608695</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20">
       <c r="A70" s="1">
         <v>218</v>
       </c>
       <c r="B70" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C70">
         <v>10012</v>
       </c>
       <c r="D70" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E70" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F70">
         <v>14.2</v>
@@ -5063,7 +5189,7 @@
         <v>36418</v>
       </c>
       <c r="J70" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K70">
         <v>25.9376</v>
@@ -5090,21 +5216,21 @@
         <v>482013140003</v>
       </c>
     </row>
-    <row r="71" spans="1:18">
+    <row r="71" spans="1:20">
       <c r="A71" s="1">
         <v>221</v>
       </c>
       <c r="B71" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C71">
         <v>10383</v>
       </c>
       <c r="D71" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E71" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F71">
         <v>6.3</v>
@@ -5119,7 +5245,7 @@
         <v>36586</v>
       </c>
       <c r="J71" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K71">
         <v>24.3586</v>
@@ -5146,21 +5272,21 @@
         <v>482012533001</v>
       </c>
     </row>
-    <row r="72" spans="1:18">
+    <row r="72" spans="1:20">
       <c r="A72" s="1">
         <v>224</v>
       </c>
       <c r="B72" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C72">
         <v>10182</v>
       </c>
       <c r="D72" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E72" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F72">
         <v>27.8</v>
@@ -5175,7 +5301,7 @@
         <v>36472</v>
       </c>
       <c r="J72" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K72">
         <v>23.0495</v>
@@ -5201,22 +5327,28 @@
       <c r="R72">
         <v>482012533002</v>
       </c>
-    </row>
-    <row r="73" spans="1:18">
+      <c r="S72">
+        <v>29.758572912</v>
+      </c>
+      <c r="T72">
+        <v>-95.06787043999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20">
       <c r="A73" s="1">
         <v>227</v>
       </c>
       <c r="B73" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C73">
         <v>10149</v>
       </c>
       <c r="D73" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E73" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F73">
         <v>29.4</v>
@@ -5231,7 +5363,7 @@
         <v>36472</v>
       </c>
       <c r="J73" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K73">
         <v>23.8209</v>
@@ -5258,21 +5390,21 @@
         <v>482012535004</v>
       </c>
     </row>
-    <row r="74" spans="1:18">
+    <row r="74" spans="1:20">
       <c r="A74" s="1">
         <v>230</v>
       </c>
       <c r="B74" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C74">
         <v>10155</v>
       </c>
       <c r="D74" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E74" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F74">
         <v>16.1</v>
@@ -5287,7 +5419,7 @@
         <v>36479</v>
       </c>
       <c r="J74" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K74">
         <v>22.5091</v>
@@ -5314,21 +5446,21 @@
         <v>482012537001</v>
       </c>
     </row>
-    <row r="75" spans="1:18">
+    <row r="75" spans="1:20">
       <c r="A75" s="1">
         <v>236</v>
       </c>
       <c r="B75" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C75">
         <v>10180</v>
       </c>
       <c r="D75" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E75" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F75">
         <v>42.3</v>
@@ -5343,7 +5475,7 @@
         <v>36493</v>
       </c>
       <c r="J75" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K75">
         <v>0</v>
@@ -5370,21 +5502,21 @@
         <v>482013223001</v>
       </c>
     </row>
-    <row r="76" spans="1:18">
+    <row r="76" spans="1:20">
       <c r="A76" s="1">
         <v>239</v>
       </c>
       <c r="B76" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C76">
         <v>10035</v>
       </c>
       <c r="D76" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E76" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F76">
         <v>16.1</v>
@@ -5399,7 +5531,7 @@
         <v>36486</v>
       </c>
       <c r="J76" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K76">
         <v>25.9881</v>
@@ -5426,21 +5558,21 @@
         <v>482013223001</v>
       </c>
     </row>
-    <row r="77" spans="1:18">
+    <row r="77" spans="1:20">
       <c r="A77" s="1">
         <v>242</v>
       </c>
       <c r="B77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C77">
         <v>10029</v>
       </c>
       <c r="D77" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E77" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F77">
         <v>29</v>
@@ -5455,7 +5587,7 @@
         <v>36515</v>
       </c>
       <c r="J77" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K77">
         <v>18.4841</v>
@@ -5482,21 +5614,21 @@
         <v>482013223001</v>
       </c>
     </row>
-    <row r="78" spans="1:18">
+    <row r="78" spans="1:20">
       <c r="A78" s="1">
         <v>245</v>
       </c>
       <c r="B78" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C78">
         <v>10185</v>
       </c>
       <c r="D78" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E78" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F78">
         <v>27</v>
@@ -5511,7 +5643,7 @@
         <v>36493</v>
       </c>
       <c r="J78" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K78">
         <v>22.8939</v>
@@ -5538,21 +5670,21 @@
         <v>482013223001</v>
       </c>
     </row>
-    <row r="79" spans="1:18">
+    <row r="79" spans="1:20">
       <c r="A79" s="1">
         <v>248</v>
       </c>
       <c r="B79" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C79">
         <v>10281</v>
       </c>
       <c r="D79" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E79" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F79">
         <v>10.7</v>
@@ -5567,7 +5699,7 @@
         <v>36538</v>
       </c>
       <c r="J79" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K79">
         <v>22.3189</v>
@@ -5594,21 +5726,21 @@
         <v>482013223001</v>
       </c>
     </row>
-    <row r="80" spans="1:18">
+    <row r="80" spans="1:20">
       <c r="A80" s="1">
         <v>251</v>
       </c>
       <c r="B80" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C80">
         <v>10346</v>
       </c>
       <c r="D80" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E80" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F80">
         <v>34.5</v>
@@ -5623,7 +5755,7 @@
         <v>36536</v>
       </c>
       <c r="J80" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K80">
         <v>26.6618</v>
@@ -5650,21 +5782,21 @@
         <v>482013223001</v>
       </c>
     </row>
-    <row r="81" spans="1:18">
+    <row r="81" spans="1:20">
       <c r="A81" s="1">
         <v>254</v>
       </c>
       <c r="B81" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C81">
         <v>10254</v>
       </c>
       <c r="D81" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E81" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F81">
         <v>32</v>
@@ -5679,7 +5811,7 @@
         <v>36556</v>
       </c>
       <c r="J81" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K81">
         <v>19.1203</v>
@@ -5706,21 +5838,21 @@
         <v>482013219004</v>
       </c>
     </row>
-    <row r="82" spans="1:18">
+    <row r="82" spans="1:20">
       <c r="A82" s="1">
         <v>257</v>
       </c>
       <c r="B82" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C82">
         <v>10255</v>
       </c>
       <c r="D82" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E82" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F82">
         <v>8.199999999999999</v>
@@ -5735,7 +5867,7 @@
         <v>36556</v>
       </c>
       <c r="J82" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K82">
         <v>22.1981</v>
@@ -5762,21 +5894,21 @@
         <v>482013238002</v>
       </c>
     </row>
-    <row r="83" spans="1:18">
+    <row r="83" spans="1:20">
       <c r="A83" s="1">
         <v>260</v>
       </c>
       <c r="B83" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C83">
         <v>10385</v>
       </c>
       <c r="D83" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E83" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F83">
         <v>29.7</v>
@@ -5791,7 +5923,7 @@
         <v>36595</v>
       </c>
       <c r="J83" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K83">
         <v>22.2767</v>
@@ -5818,21 +5950,21 @@
         <v>482013223001</v>
       </c>
     </row>
-    <row r="84" spans="1:18">
+    <row r="84" spans="1:20">
       <c r="A84" s="1">
         <v>267</v>
       </c>
       <c r="B84" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C84">
         <v>10648</v>
       </c>
       <c r="D84" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E84" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F84">
         <v>4.4</v>
@@ -5847,7 +5979,7 @@
         <v>36698</v>
       </c>
       <c r="J84" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K84">
         <v>0</v>
@@ -5874,21 +6006,21 @@
         <v>482013232003</v>
       </c>
     </row>
-    <row r="85" spans="1:18">
+    <row r="85" spans="1:20">
       <c r="A85" s="1">
         <v>270</v>
       </c>
       <c r="B85" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C85">
         <v>10670</v>
       </c>
       <c r="D85" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E85" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F85">
         <v>5.5</v>
@@ -5903,7 +6035,7 @@
         <v>36703</v>
       </c>
       <c r="J85" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K85">
         <v>0</v>
@@ -5930,21 +6062,21 @@
         <v>482012337007</v>
       </c>
     </row>
-    <row r="86" spans="1:18">
+    <row r="86" spans="1:20">
       <c r="A86" s="1">
         <v>273</v>
       </c>
       <c r="B86" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C86">
         <v>10645</v>
       </c>
       <c r="D86" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E86" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F86">
         <v>7.2</v>
@@ -5959,7 +6091,7 @@
         <v>36698</v>
       </c>
       <c r="J86" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K86">
         <v>25.1701</v>
@@ -5986,21 +6118,21 @@
         <v>482012337002</v>
       </c>
     </row>
-    <row r="87" spans="1:18">
+    <row r="87" spans="1:20">
       <c r="A87" s="1">
         <v>276</v>
       </c>
       <c r="B87" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C87">
         <v>10680</v>
       </c>
       <c r="D87" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E87" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F87">
         <v>5.7</v>
@@ -6015,7 +6147,7 @@
         <v>36719</v>
       </c>
       <c r="J87" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K87">
         <v>0</v>
@@ -6042,21 +6174,21 @@
         <v>482012539001</v>
       </c>
     </row>
-    <row r="88" spans="1:18">
+    <row r="88" spans="1:20">
       <c r="A88" s="1">
         <v>279</v>
       </c>
       <c r="B88" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C88">
         <v>10683</v>
       </c>
       <c r="D88" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E88" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F88">
         <v>4.8</v>
@@ -6071,7 +6203,7 @@
         <v>36724</v>
       </c>
       <c r="J88" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K88">
         <v>23.89</v>
@@ -6098,21 +6230,21 @@
         <v>482012533003</v>
       </c>
     </row>
-    <row r="89" spans="1:18">
+    <row r="89" spans="1:20">
       <c r="A89" s="1">
         <v>282</v>
       </c>
       <c r="B89" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C89">
         <v>10669</v>
       </c>
       <c r="D89" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E89" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F89">
         <v>5.4</v>
@@ -6127,7 +6259,7 @@
         <v>36712</v>
       </c>
       <c r="J89" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K89">
         <v>24.8747</v>
@@ -6154,21 +6286,21 @@
         <v>480717102002</v>
       </c>
     </row>
-    <row r="90" spans="1:18">
+    <row r="90" spans="1:20">
       <c r="A90" s="1">
         <v>283</v>
       </c>
       <c r="B90" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C90">
         <v>10669</v>
       </c>
       <c r="D90" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E90" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F90">
         <v>5.4</v>
@@ -6183,7 +6315,7 @@
         <v>36712</v>
       </c>
       <c r="J90" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K90">
         <v>24.8747</v>
@@ -6210,21 +6342,21 @@
         <v>480717102002</v>
       </c>
     </row>
-    <row r="91" spans="1:18">
+    <row r="91" spans="1:20">
       <c r="A91" s="1">
         <v>288</v>
       </c>
       <c r="B91" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C91">
         <v>10679</v>
       </c>
       <c r="D91" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E91" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F91">
         <v>4</v>
@@ -6239,7 +6371,7 @@
         <v>36719</v>
       </c>
       <c r="J91" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K91">
         <v>25.6</v>
@@ -6266,21 +6398,21 @@
         <v>480717102002</v>
       </c>
     </row>
-    <row r="92" spans="1:18">
+    <row r="92" spans="1:20">
       <c r="A92" s="1">
         <v>297</v>
       </c>
       <c r="B92" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C92">
         <v>10771</v>
       </c>
       <c r="D92" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E92" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F92">
         <v>9</v>
@@ -6295,7 +6427,7 @@
         <v>36733</v>
       </c>
       <c r="J92" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K92">
         <v>23.9</v>
@@ -6310,21 +6442,21 @@
         <v>482012545001</v>
       </c>
     </row>
-    <row r="93" spans="1:18">
+    <row r="93" spans="1:20">
       <c r="A93" s="1">
         <v>303</v>
       </c>
       <c r="B93" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C93">
         <v>10766</v>
       </c>
       <c r="D93" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E93" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F93">
         <v>15.9</v>
@@ -6339,7 +6471,7 @@
         <v>36731</v>
       </c>
       <c r="J93" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K93">
         <v>29.5</v>
@@ -6366,21 +6498,21 @@
         <v>482012534001</v>
       </c>
     </row>
-    <row r="94" spans="1:18">
+    <row r="94" spans="1:20">
       <c r="A94" s="1">
         <v>306</v>
       </c>
       <c r="B94" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C94">
         <v>10773</v>
       </c>
       <c r="D94" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E94" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F94">
         <v>10.3</v>
@@ -6395,7 +6527,7 @@
         <v>36738</v>
       </c>
       <c r="J94" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K94">
         <v>0</v>
@@ -6422,21 +6554,21 @@
         <v>482013203001</v>
       </c>
     </row>
-    <row r="95" spans="1:18">
+    <row r="95" spans="1:20">
       <c r="A95" s="1">
         <v>309</v>
       </c>
       <c r="B95" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C95">
         <v>10955</v>
       </c>
       <c r="D95" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E95" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F95">
         <v>3.6</v>
@@ -6451,7 +6583,7 @@
         <v>36837</v>
       </c>
       <c r="J95" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K95">
         <v>24.1246</v>
@@ -6478,21 +6610,21 @@
         <v>482012523003</v>
       </c>
     </row>
-    <row r="96" spans="1:18">
+    <row r="96" spans="1:20">
       <c r="A96" s="1">
         <v>312</v>
       </c>
       <c r="B96" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C96">
         <v>10749</v>
       </c>
       <c r="D96" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E96" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F96">
         <v>10.3</v>
@@ -6507,7 +6639,7 @@
         <v>36740</v>
       </c>
       <c r="J96" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K96">
         <v>0</v>
@@ -6533,22 +6665,28 @@
       <c r="R96">
         <v>482012524002</v>
       </c>
-    </row>
-    <row r="97" spans="1:18">
+      <c r="S96">
+        <v>29.78980206</v>
+      </c>
+      <c r="T96">
+        <v>-95.16006806</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20">
       <c r="A97" s="1">
         <v>315</v>
       </c>
       <c r="B97" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C97">
         <v>10813</v>
       </c>
       <c r="D97" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E97" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F97">
         <v>16.7</v>
@@ -6563,7 +6701,7 @@
         <v>36747</v>
       </c>
       <c r="J97" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K97">
         <v>28.1</v>
@@ -6589,22 +6727,28 @@
       <c r="R97">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="98" spans="1:18">
+      <c r="S97">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T97">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20">
       <c r="A98" s="1">
         <v>318</v>
       </c>
       <c r="B98" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C98">
         <v>10818</v>
       </c>
       <c r="D98" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E98" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F98">
         <v>4.3</v>
@@ -6619,7 +6763,7 @@
         <v>36752</v>
       </c>
       <c r="J98" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K98">
         <v>0</v>
@@ -6645,22 +6789,28 @@
       <c r="R98">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="99" spans="1:18">
+      <c r="S98">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T98">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20">
       <c r="A99" s="1">
         <v>321</v>
       </c>
       <c r="B99" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C99">
         <v>10820</v>
       </c>
       <c r="D99" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E99" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F99">
         <v>9.4</v>
@@ -6675,7 +6825,7 @@
         <v>36752</v>
       </c>
       <c r="J99" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K99">
         <v>0</v>
@@ -6701,22 +6851,28 @@
       <c r="R99">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="100" spans="1:18">
+      <c r="S99">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T99">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20">
       <c r="A100" s="1">
         <v>324</v>
       </c>
       <c r="B100" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C100">
         <v>10814</v>
       </c>
       <c r="D100" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E100" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F100">
         <v>25.3</v>
@@ -6731,7 +6887,7 @@
         <v>36745</v>
       </c>
       <c r="J100" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K100">
         <v>23.9</v>
@@ -6757,22 +6913,28 @@
       <c r="R100">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="101" spans="1:18">
+      <c r="S100">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T100">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20">
       <c r="A101" s="1">
         <v>327</v>
       </c>
       <c r="B101" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C101">
         <v>10816</v>
       </c>
       <c r="D101" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E101" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F101">
         <v>4.3</v>
@@ -6787,7 +6949,7 @@
         <v>36747</v>
       </c>
       <c r="J101" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K101">
         <v>0</v>
@@ -6814,21 +6976,21 @@
         <v>482012330004</v>
       </c>
     </row>
-    <row r="102" spans="1:18">
+    <row r="102" spans="1:20">
       <c r="A102" s="1">
         <v>330</v>
       </c>
       <c r="B102" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C102">
         <v>10748</v>
       </c>
       <c r="D102" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E102" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F102">
         <v>5.9</v>
@@ -6843,7 +7005,7 @@
         <v>36740</v>
       </c>
       <c r="J102" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K102">
         <v>25.6</v>
@@ -6870,21 +7032,21 @@
         <v>482012523002</v>
       </c>
     </row>
-    <row r="103" spans="1:18">
+    <row r="103" spans="1:20">
       <c r="A103" s="1">
         <v>333</v>
       </c>
       <c r="B103" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C103">
         <v>10890</v>
       </c>
       <c r="D103" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E103" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F103">
         <v>15.9</v>
@@ -6899,7 +7061,7 @@
         <v>36788</v>
       </c>
       <c r="J103" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K103">
         <v>26.7</v>
@@ -6926,21 +7088,21 @@
         <v>482012526001</v>
       </c>
     </row>
-    <row r="104" spans="1:18">
+    <row r="104" spans="1:20">
       <c r="A104" s="1">
         <v>336</v>
       </c>
       <c r="B104" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C104">
         <v>10891</v>
       </c>
       <c r="D104" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E104" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F104">
         <v>7.5</v>
@@ -6955,7 +7117,7 @@
         <v>36788</v>
       </c>
       <c r="J104" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K104">
         <v>27.2</v>
@@ -6982,21 +7144,21 @@
         <v>482012526001</v>
       </c>
     </row>
-    <row r="105" spans="1:18">
+    <row r="105" spans="1:20">
       <c r="A105" s="1">
         <v>338</v>
       </c>
       <c r="B105" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C105">
         <v>10829</v>
       </c>
       <c r="D105" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E105" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F105">
         <v>25.3</v>
@@ -7011,7 +7173,7 @@
         <v>36754</v>
       </c>
       <c r="J105" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K105">
         <v>26.7</v>
@@ -7037,22 +7199,28 @@
       <c r="R105">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="106" spans="1:18">
+      <c r="S105">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T105">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20">
       <c r="A106" s="1">
         <v>341</v>
       </c>
       <c r="B106" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C106">
         <v>10871</v>
       </c>
       <c r="D106" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E106" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F106">
         <v>31.9</v>
@@ -7067,7 +7235,7 @@
         <v>36761</v>
       </c>
       <c r="J106" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K106">
         <v>28.1</v>
@@ -7093,22 +7261,28 @@
       <c r="R106">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="107" spans="1:18">
+      <c r="S106">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T106">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20">
       <c r="A107" s="1">
         <v>344</v>
       </c>
       <c r="B107" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C107">
         <v>10828</v>
       </c>
       <c r="D107" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E107" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F107">
         <v>12.3</v>
@@ -7123,7 +7297,7 @@
         <v>36754</v>
       </c>
       <c r="J107" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K107">
         <v>0</v>
@@ -7149,22 +7323,28 @@
       <c r="R107">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="108" spans="1:18">
+      <c r="S107">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T107">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20">
       <c r="A108" s="1">
         <v>347</v>
       </c>
       <c r="B108" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C108">
         <v>10826</v>
       </c>
       <c r="D108" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E108" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F108">
         <v>5.3</v>
@@ -7179,7 +7359,7 @@
         <v>36759</v>
       </c>
       <c r="J108" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K108">
         <v>23.9</v>
@@ -7206,21 +7386,21 @@
         <v>482012526001</v>
       </c>
     </row>
-    <row r="109" spans="1:18">
+    <row r="109" spans="1:20">
       <c r="A109" s="1">
         <v>350</v>
       </c>
       <c r="B109" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C109">
         <v>10824</v>
       </c>
       <c r="D109" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E109" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F109">
         <v>9.9</v>
@@ -7235,7 +7415,7 @@
         <v>36759</v>
       </c>
       <c r="J109" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K109">
         <v>25.6</v>
@@ -7262,21 +7442,21 @@
         <v>482012526001</v>
       </c>
     </row>
-    <row r="110" spans="1:18">
+    <row r="110" spans="1:20">
       <c r="A110" s="1">
         <v>351</v>
       </c>
       <c r="B110" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C110">
         <v>10824</v>
       </c>
       <c r="D110" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E110" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F110">
         <v>9.9</v>
@@ -7291,7 +7471,7 @@
         <v>36759</v>
       </c>
       <c r="J110" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K110">
         <v>25.6</v>
@@ -7318,21 +7498,21 @@
         <v>482012526001</v>
       </c>
     </row>
-    <row r="111" spans="1:18">
+    <row r="111" spans="1:20">
       <c r="A111" s="1">
         <v>356</v>
       </c>
       <c r="B111" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C111">
         <v>10953</v>
       </c>
       <c r="D111" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E111" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F111">
         <v>27</v>
@@ -7347,7 +7527,7 @@
         <v>36816</v>
       </c>
       <c r="J111" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K111">
         <v>21.7</v>
@@ -7373,22 +7553,28 @@
       <c r="R111">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="112" spans="1:18">
+      <c r="S111">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T111">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="112" spans="1:20">
       <c r="A112" s="1">
         <v>359</v>
       </c>
       <c r="B112" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C112">
         <v>10885</v>
       </c>
       <c r="D112" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E112" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F112">
         <v>46.1</v>
@@ -7403,7 +7589,7 @@
         <v>36832</v>
       </c>
       <c r="J112" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K112">
         <v>26.3974</v>
@@ -7429,22 +7615,28 @@
       <c r="R112">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="113" spans="1:18">
+      <c r="S112">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T112">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20">
       <c r="A113" s="1">
         <v>362</v>
       </c>
       <c r="B113" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C113">
         <v>10962</v>
       </c>
       <c r="D113" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E113" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F113">
         <v>31.4</v>
@@ -7459,7 +7651,7 @@
         <v>36844</v>
       </c>
       <c r="J113" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K113">
         <v>0</v>
@@ -7485,22 +7677,28 @@
       <c r="R113">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="114" spans="1:18">
+      <c r="S113">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T113">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20">
       <c r="A114" s="1">
         <v>368</v>
       </c>
       <c r="B114" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C114">
         <v>10899</v>
       </c>
       <c r="D114" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E114" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F114">
         <v>78.90000000000001</v>
@@ -7515,7 +7713,7 @@
         <v>36781</v>
       </c>
       <c r="J114" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K114">
         <v>26.7</v>
@@ -7539,21 +7737,21 @@
         <v>88.24116666666667</v>
       </c>
     </row>
-    <row r="115" spans="1:18">
+    <row r="115" spans="1:20">
       <c r="A115" s="1">
         <v>370</v>
       </c>
       <c r="B115" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C115">
         <v>10881</v>
       </c>
       <c r="D115" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E115" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F115">
         <v>33.7</v>
@@ -7568,7 +7766,7 @@
         <v>36774</v>
       </c>
       <c r="J115" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K115">
         <v>28.1</v>
@@ -7594,22 +7792,28 @@
       <c r="R115">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="116" spans="1:18">
+      <c r="S115">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T115">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20">
       <c r="A116" s="1">
         <v>373</v>
       </c>
       <c r="B116" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C116">
         <v>10875</v>
       </c>
       <c r="D116" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F116">
         <v>10.8</v>
@@ -7624,7 +7828,7 @@
         <v>36766</v>
       </c>
       <c r="J116" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K116">
         <v>25.3</v>
@@ -7650,22 +7854,28 @@
       <c r="R116">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="117" spans="1:18">
+      <c r="S116">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T116">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="117" spans="1:20">
       <c r="A117" s="1">
         <v>376</v>
       </c>
       <c r="B117" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C117">
         <v>10895</v>
       </c>
       <c r="D117" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E117" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F117">
         <v>13.4</v>
@@ -7680,7 +7890,7 @@
         <v>36802</v>
       </c>
       <c r="J117" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K117">
         <v>23.9</v>
@@ -7706,22 +7916,28 @@
       <c r="R117">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="118" spans="1:18">
+      <c r="S117">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T117">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20">
       <c r="A118" s="1">
         <v>379</v>
       </c>
       <c r="B118" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C118">
         <v>10870</v>
       </c>
       <c r="D118" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E118" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F118">
         <v>27</v>
@@ -7736,7 +7952,7 @@
         <v>36761</v>
       </c>
       <c r="J118" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K118">
         <v>26.9</v>
@@ -7762,22 +7978,28 @@
       <c r="R118">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="119" spans="1:18">
+      <c r="S118">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T118">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20">
       <c r="A119" s="1">
         <v>384</v>
       </c>
       <c r="B119" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C119">
         <v>10900</v>
       </c>
       <c r="D119" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E119" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F119">
         <v>10.8</v>
@@ -7792,7 +8014,7 @@
         <v>36781</v>
       </c>
       <c r="J119" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K119">
         <v>15.56</v>
@@ -7819,21 +8041,21 @@
         <v>482012526001</v>
       </c>
     </row>
-    <row r="120" spans="1:18">
+    <row r="120" spans="1:20">
       <c r="A120" s="1">
         <v>386</v>
       </c>
       <c r="B120" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C120">
         <v>10879</v>
       </c>
       <c r="D120" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E120" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F120">
         <v>9</v>
@@ -7848,7 +8070,7 @@
         <v>36768</v>
       </c>
       <c r="J120" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K120">
         <v>25.3</v>
@@ -7862,22 +8084,28 @@
       <c r="R120">
         <v>482012526004</v>
       </c>
-    </row>
-    <row r="121" spans="1:18">
+      <c r="S120">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T120">
+        <v>-95.0968974625</v>
+      </c>
+    </row>
+    <row r="121" spans="1:20">
       <c r="A121" s="1">
         <v>389</v>
       </c>
       <c r="B121" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C121">
         <v>10877</v>
       </c>
       <c r="D121" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E121" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F121">
         <v>15.6</v>
@@ -7892,7 +8120,7 @@
         <v>36768</v>
       </c>
       <c r="J121" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K121">
         <v>25.3</v>
@@ -7905,6 +8133,12 @@
       </c>
       <c r="R121">
         <v>482012526004</v>
+      </c>
+      <c r="S121">
+        <v>29.7877019125</v>
+      </c>
+      <c r="T121">
+        <v>-95.0968974625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>